<commit_message>
reversed sorting in g12cnn and g12dnn, finalized exporting data in a nice .xlsx file
</commit_message>
<xml_diff>
--- a/Quality of Life/list_for_Risha.xlsx
+++ b/Quality of Life/list_for_Risha.xlsx
@@ -1215,129 +1215,147 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CHEMBL1184</t>
+          <t>CHEMBL1200728</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ACETYLCHOLINE CHLORIDE</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr"/>
+          <t>GUANIDINE HYDROCHLORIDE</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>10.190047</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>CHEMBL730</t>
+          <t>CHEMBL2107067</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>NITROGLYCERIN</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr"/>
+          <t>TESTOSTERONE UNDECANOATE</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>7.7600026</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>CHEMBL2110948</t>
+          <t>CHEMBL1371</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>POLDINE</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr"/>
+          <t>CHLORZOXAZONE</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>7.4483685</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>CHEMBL1201264</t>
+          <t>CHEMBL492</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>METHANTHELINE</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr"/>
+          <t>ETIDOCAINE</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>5.872513</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>CHEMBL1401367</t>
+          <t>CHEMBL878</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>PIPENZOLATE BROMIDE</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr"/>
+          <t>METOLAZONE</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>5.800352</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CHEMBL1200829</t>
+          <t>CHEMBL1529</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>GLUCONOLACTONE</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr"/>
+          <t>DIPHENIDOL HYDROCHLORIDE</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>5.622511</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>CHEMBL1201336</t>
+          <t>CHEMBL1200410</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>FOSPHENYTOIN</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr"/>
+          <t>PROCARBAZINE HYDROCHLORIDE</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>5.469802</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>CHEMBL404422</t>
+          <t>CHEMBL5315118</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>BUTETHAL</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr"/>
+          <t>ILOPROST TROMETHAMINE</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>4.2749567</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>CHEMBL1401</t>
+          <t>CHEMBL730</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>NITAZOXANIDE</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr"/>
+          <t>NITROGLYCERIN</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>3.3668554</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>CHEMBL1411731</t>
+          <t>CHEMBL1200968</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>TALAMPICILLIN HYDROCHLORIDE</t>
+          <t>HYDROCORTISONE SODIUM PHOSPHATE</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
@@ -1345,12 +1363,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>CHEMBL1200398</t>
+          <t>CHEMBL1371200</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>BUTOCONAZOLE NITRATE</t>
+          <t>CANRENOATE POTASSIUM</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
@@ -1392,167 +1410,161 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>CHEMBL1318287</t>
+          <t>CHEMBL4303454</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>PENTOLINIUM TARTRATE</t>
+          <t>DORIPENEM MONOHYDRATE</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>1.7297717</v>
+        <v>6.483579</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>CHEMBL1577</t>
+          <t>CHEMBL1200635</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>METHYCLOTHIAZIDE</t>
+          <t>HYDROCORTAMATE HYDROCHLORIDE</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>2.4957638</v>
+        <v>6.2385273</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CHEMBL730</t>
+          <t>CHEMBL2107067</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>NITROGLYCERIN</t>
+          <t>TESTOSTERONE UNDECANOATE</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>2.5334873</v>
+        <v>5.975186</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>CHEMBL435</t>
+          <t>CHEMBL492</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>HYDROCHLOROTHIAZIDE</t>
+          <t>ETIDOCAINE</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>2.556745</v>
+        <v>5.768978</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>CHEMBL3545313</t>
+          <t>CHEMBL878</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>BEMPEDOIC ACID</t>
+          <t>METOLAZONE</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>2.6054378</v>
+        <v>5.024636</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>CHEMBL1243</t>
+          <t>CHEMBL1529</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>SULFABENZAMIDE</t>
+          <t>DIPHENIDOL HYDROCHLORIDE</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>2.6374588</v>
+        <v>4.085992</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>CHEMBL404422</t>
+          <t>CHEMBL5315118</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>BUTETHAL</t>
+          <t>ILOPROST TROMETHAMINE</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>2.9931388</v>
+        <v>3.448734</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>CHEMBL1455</t>
+          <t>CHEMBL730</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>ALTRETAMINE</t>
+          <t>NITROGLYCERIN</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>3.099568</v>
+        <v>3.1568189</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>CHEMBL2111157</t>
+          <t>CHEMBL1200968</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DIPIPANONE</t>
-        </is>
-      </c>
-      <c r="C73" t="n">
-        <v>3.1700957</v>
-      </c>
+          <t>HYDROCORTISONE SODIUM PHOSPHATE</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>CHEMBL1524273</t>
+          <t>CHEMBL1371200</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>PHTHALYLSULFATHIAZOLE</t>
-        </is>
-      </c>
-      <c r="C74" t="n">
-        <v>3.1897159</v>
-      </c>
+          <t>CANRENOATE POTASSIUM</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>CHEMBL61593</t>
+          <t>CHEMBL1200487</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>CYCLOTHIAZIDE</t>
-        </is>
-      </c>
-      <c r="C75" t="n">
-        <v>3.3447206</v>
-      </c>
+          <t>ETHACRYNATE SODIUM</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">

</xml_diff>